<commit_message>
added test data in excel
</commit_message>
<xml_diff>
--- a/RestAssuredBDD-GoRestAPI_Automation/src/main/java/Resources/TestData.xlsx
+++ b/RestAssuredBDD-GoRestAPI_Automation/src/main/java/Resources/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Test Create User API</t>
+  </si>
+  <si>
+    <t>Test Edit User details API</t>
   </si>
 </sst>
 </file>
@@ -408,17 +411,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -446,7 +449,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>8070403</v>
+        <v>8107043</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -480,6 +483,15 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>8106977</v>
+      </c>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>